<commit_message>
Slight change to the excel file with data plots
</commit_message>
<xml_diff>
--- a/trial_results_final.xlsx
+++ b/trial_results_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Scheduling_with_RL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DF03F58A-48D2-4067-9B21-D1754EAF7E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0353251A-71BD-43CF-B225-2588D1AD1718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="trial_results_final" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +582,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -641,358 +642,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65%"/>
-                  <a:lumOff val="35%"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Queue Time as % of Oracle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75%"/>
-                        <a:lumOff val="25%"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35%"/>
-                          <a:lumOff val="65%"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Oracle</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Best Bin First</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PPO Agent 5k</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>PPO Agent 3M</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1423170101230509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.211913772228236</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2759796736137208</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B925-4321-941B-0A510FF90D6F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="981448944"/>
-        <c:axId val="981448464"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="981448944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15%"/>
-                <a:lumOff val="85%"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65%"/>
-                    <a:lumOff val="35%"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981448464"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="981448464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15%"/>
-                  <a:lumOff val="85%"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65%"/>
-                    <a:lumOff val="35%"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981448944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15%"/>
-          <a:lumOff val="85%"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1345,6 +994,710 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Queue Time (sec)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75%"/>
+                        <a:lumOff val="25%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35%"/>
+                          <a:lumOff val="65%"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Oracle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Best Bin First</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PPO Agent 5k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PPO Agent 3M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26007.416799999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29708.714599999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31518.746599999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33184.9352</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7133-4004-9CC7-B5E9004DE6F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="981448944"/>
+        <c:axId val="981448464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="981448944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15%"/>
+                <a:lumOff val="85%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981448464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981448464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981448944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Queue Time as % of Oracle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75%"/>
+                        <a:lumOff val="25%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35%"/>
+                          <a:lumOff val="65%"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Oracle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Best Bin First</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PPO Agent 5k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PPO Agent 3M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1423170101230509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.211913772228236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2759796736137208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B925-4321-941B-0A510FF90D6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="981448944"/>
+        <c:axId val="981448464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="981448944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15%"/>
+                <a:lumOff val="85%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981448464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981448464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981448944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1425,6 +1778,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="201">
   <cs:axisTitle>
@@ -2431,8 +2824,585 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65%"/>
+          <a:lumOff val="35%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75%"/>
+            <a:lumOff val="25%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2D006B-6DA3-5BCD-BAF2-B96B4A67EF4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03655D3C-E009-4790-BF6A-E273F78B4B09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2463,43 +3433,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
-          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2D006B-6DA3-5BCD-BAF2-B96B4A67EF4E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
-          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2807,9 +3741,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3251,7 +4183,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3278,7 +4212,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>26007.416799999999</v>
       </c>
       <c r="C2" s="4">
@@ -3293,7 +4227,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>29708.714599999999</v>
       </c>
       <c r="C3" s="4">
@@ -3308,7 +4242,7 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>31518.746599999999</v>
       </c>
       <c r="C4" s="4">
@@ -3323,7 +4257,7 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>33184.9352</v>
       </c>
       <c r="C5" s="4">

</xml_diff>

<commit_message>
Did 20 trials overnight for more data
</commit_message>
<xml_diff>
--- a/trial_results_final.xlsx
+++ b/trial_results_final.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Scheduling_with_RL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0353251A-71BD-43CF-B225-2588D1AD1718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8B476561-096F-45BB-8F41-B4EEA4403B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trial_results_final" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="plots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -574,15 +574,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -697,7 +697,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>plots!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -776,7 +776,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>plots!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -796,7 +796,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>plots!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1050,7 +1050,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>plots!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1129,7 +1129,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>plots!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1149,7 +1149,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>plots!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1402,7 +1402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>plots!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1481,7 +1481,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>plots!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1501,7 +1501,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:f>plots!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3331,16 +3331,16 @@
 <xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3367,16 +3367,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>592455</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3405,16 +3405,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3738,41 +3738,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3808,12 +3808,12 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <f>AVERAGE(D7:D11)</f>
         <v>399.93320000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3829,9 +3829,9 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3847,9 +3847,9 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3865,9 +3865,9 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3883,9 +3883,9 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3901,12 +3901,12 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="5">
         <f>AVERAGE(D12:D16)</f>
         <v>421.54879999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3922,9 +3922,9 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3940,9 +3940,9 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -3958,9 +3958,9 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3976,9 +3976,9 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3994,12 +3994,12 @@
       <c r="E17">
         <v>24128</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="5">
         <f>AVERAGE(D17:D21)</f>
         <v>415.81040000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4015,9 +4015,9 @@
       <c r="E18">
         <v>24128</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -4033,9 +4033,9 @@
       <c r="E19">
         <v>24128</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4051,9 +4051,9 @@
       <c r="E20">
         <v>24128</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -4069,9 +4069,9 @@
       <c r="E21">
         <v>24128</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -4087,12 +4087,12 @@
       <c r="E22">
         <v>34268</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="5">
         <f>AVERAGE(D22:D26)</f>
         <v>420.39279999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4108,9 +4108,9 @@
       <c r="E23">
         <v>34268</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -4126,9 +4126,9 @@
       <c r="E24">
         <v>34268</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -4144,9 +4144,9 @@
       <c r="E25">
         <v>34268</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4162,7 +4162,7 @@
       <c r="E26">
         <v>34268</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E26">
@@ -4180,90 +4180,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>26007.416799999999</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>421.54879999999991</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>B2/$B$2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>29708.714599999999</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>399.93320000000006</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D5" si="0">B3/$B$2</f>
         <v>1.1423170101230509</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>31518.746599999999</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>420.39279999999997</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>1.211913772228236</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>33184.9352</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>415.81040000000002</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>1.2759796736137208</v>
       </c>

</xml_diff>